<commit_message>
fix Lm data, add data limited Lm
</commit_message>
<xml_diff>
--- a/AdultMaturityList.xlsx
+++ b/AdultMaturityList.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwalsh/RangeShiftV2/Version3/Version4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan.morse\Documents\GitHub\NEhabitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9A3DCD-5C5E-7D4D-B71B-B9FFC143E26D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28640" windowHeight="15660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28635" windowHeight="15660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Lophius americanus</t>
   </si>
@@ -371,7 +370,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -776,22 +775,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:D83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -805,7 +804,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>50</v>
       </c>
@@ -819,7 +818,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
@@ -833,7 +832,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -847,7 +846,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -861,7 +860,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
@@ -875,7 +874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>67</v>
       </c>
@@ -889,7 +888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -903,7 +902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -917,7 +916,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -931,7 +930,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
@@ -945,7 +944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -959,7 +958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -973,7 +972,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -987,7 +986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -1001,7 +1000,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>56</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -1029,7 +1028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>61</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -1169,7 +1168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
@@ -1197,7 +1196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>83</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
@@ -1225,7 +1224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>81</v>
       </c>
@@ -1253,7 +1252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>52</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>48</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>80</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>58</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>0</v>
       </c>
@@ -1379,584 +1378,253 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="10">
-        <v>15</v>
-      </c>
-      <c r="D43" s="11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="11">
-        <v>22</v>
-      </c>
-      <c r="D44" s="11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="11">
-        <v>23</v>
-      </c>
-      <c r="D45" s="11">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="11">
-        <v>24</v>
-      </c>
-      <c r="D46" s="11">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="11">
-        <v>25</v>
-      </c>
-      <c r="D47" s="11">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="11">
-        <v>26</v>
-      </c>
-      <c r="D48" s="11">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="11">
-        <v>27</v>
-      </c>
-      <c r="D49" s="11">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="11">
-        <v>28</v>
-      </c>
-      <c r="D50" s="11">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="10">
-        <v>32</v>
-      </c>
-      <c r="D51" s="12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" s="10">
-        <v>69</v>
-      </c>
-      <c r="D52" s="12">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="10">
-        <v>72</v>
-      </c>
-      <c r="D53" s="12">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="10">
-        <v>73</v>
-      </c>
-      <c r="D54" s="12">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" s="10">
-        <v>74</v>
-      </c>
-      <c r="D55" s="12">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="10">
-        <v>75</v>
-      </c>
-      <c r="D56" s="12">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="10">
-        <v>76</v>
-      </c>
-      <c r="D57" s="10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C58" s="10">
-        <v>77</v>
-      </c>
-      <c r="D58" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" s="12">
-        <v>83</v>
-      </c>
-      <c r="D59" s="12">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C60" s="10">
-        <v>84</v>
-      </c>
-      <c r="D60" s="10">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="10">
-        <v>101</v>
-      </c>
-      <c r="D61" s="10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" s="10">
-        <v>102</v>
-      </c>
-      <c r="D62" s="12">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" s="10">
-        <v>103</v>
-      </c>
-      <c r="D63" s="10">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C64" s="12">
-        <v>104</v>
-      </c>
-      <c r="D64" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" s="10">
-        <v>105</v>
-      </c>
-      <c r="D65" s="10">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C66" s="10">
-        <v>106</v>
-      </c>
-      <c r="D66" s="10">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C67" s="10">
-        <v>107</v>
-      </c>
-      <c r="D67" s="10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" s="10">
-        <v>108</v>
-      </c>
-      <c r="D68" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C69" s="12">
-        <v>109</v>
-      </c>
-      <c r="D69" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C70" s="10">
-        <v>121</v>
-      </c>
-      <c r="D70" s="12">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C71" s="10">
-        <v>131</v>
-      </c>
-      <c r="D71" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C72" s="10">
-        <v>135</v>
-      </c>
-      <c r="D72" s="12">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="10">
-        <v>136</v>
-      </c>
-      <c r="D73" s="12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74" s="10">
-        <v>141</v>
-      </c>
-      <c r="D74" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="10">
-        <v>143</v>
-      </c>
-      <c r="D75" s="10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C76" s="10">
-        <v>145</v>
-      </c>
-      <c r="D76" s="10">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C77" s="10">
-        <v>149</v>
-      </c>
-      <c r="D77" s="12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C78" s="10">
-        <v>155</v>
-      </c>
-      <c r="D78" s="12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C79" s="10">
-        <v>163</v>
-      </c>
-      <c r="D79" s="12">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C80" s="10">
-        <v>181</v>
-      </c>
-      <c r="D80" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C81" s="10">
-        <v>192</v>
-      </c>
-      <c r="D81" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C82" s="10">
-        <v>193</v>
-      </c>
-      <c r="D82" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="10">
-        <v>197</v>
-      </c>
-      <c r="D83" s="12">
-        <v>37</v>
-      </c>
+    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+    </row>
+    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81"/>
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="C82"/>
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D83">
-    <sortCondition ref="C3:C83"/>
-  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>